<commit_message>
Bugfixes & slight optimize
# Removed extra listener for interpolation
# Added alternate file loading button than the main one
# Updated window title
</commit_message>
<xml_diff>
--- a/data/FRC_20220323_202718.xlsx
+++ b/data/FRC_20220323_202718.xlsx
@@ -1258,7 +1258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{8afeee87-3f9b-4bd3-b4e2-04d6fe181d4a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{5c16b36e-b9f2-443d-b6ed-8ca0e6efda54}">
   <dimension ref="A1:IF5131"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -43025,7 +43025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{d6b89bff-235b-486c-a566-6b386118651d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{5ff5e63d-447b-43ea-9b8e-c6b02b471e63}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>